<commit_message>
mvp feature completed: AddClients
</commit_message>
<xml_diff>
--- a/P1_ShoppingCartProcess/Data/RoSADatasheet.xlsx
+++ b/P1_ShoppingCartProcess/Data/RoSADatasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\Project1\Damle_M-P1\P1_ShoppingCartProcess\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ABF306E-DF5B-428C-995A-0C621FAF6EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FA8682-CDE1-46EB-8A24-57E4EA3287C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="19800" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>eggs 12, fruit loops 4, sliced bacon 10</t>
   </si>
@@ -48,15 +48,6 @@
     <t>Safridi</t>
   </si>
   <si>
-    <t>ddolasco@email.com</t>
-  </si>
-  <si>
-    <t>stothamax@email.com</t>
-  </si>
-  <si>
-    <t>bsafridi@email.com</t>
-  </si>
-  <si>
     <t>guarana fantastica 1, rain jacket 1, salad 10</t>
   </si>
   <si>
@@ -73,6 +64,9 @@
   </si>
   <si>
     <t>list</t>
+  </si>
+  <si>
+    <t>dumblaymyhit@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -405,7 +399,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,16 +412,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -438,10 +432,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -452,7 +446,7 @@
         <v>4</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -466,10 +460,10 @@
         <v>6</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -479,11 +473,6 @@
       <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{4ED5CA6A-39C7-4993-9A3E-3404FA46A167}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{B9A885E0-542D-4E83-8F0D-99D6FAA4CEFF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>